<commit_message>
Chore: Update data types
</commit_message>
<xml_diff>
--- a/assets/data_types.xlsx
+++ b/assets/data_types.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl.localhost\Ubuntu\home\nate\excel-emulator2\tests\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl.localhost\Ubuntu\home\nate\coding\excel-emulator2\assets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2ACBE5DD-BFEF-4391-943F-D177F094530E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CDD2EDD6-A39B-43FA-ACB6-DC562E8F5BC9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="22695" windowHeight="14716" xr2:uid="{6F87B0DF-F7C3-4D20-8A30-9558F5F3947A}"/>
+    <workbookView xWindow="2543" yWindow="2543" windowWidth="16875" windowHeight="10612" xr2:uid="{6F87B0DF-F7C3-4D20-8A30-9558F5F3947A}"/>
   </bookViews>
   <sheets>
     <sheet name="test 1" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
   <si>
     <t>a</t>
   </si>
@@ -58,6 +58,9 @@
   </si>
   <si>
     <t>Formulas</t>
+  </si>
+  <si>
+    <t>Shared Formula</t>
   </si>
 </sst>
 </file>
@@ -410,18 +413,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C88686C4-D81F-4531-855F-4C83D5EE15A6}">
-  <dimension ref="A1:D4"/>
+  <dimension ref="A1:E4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L12" sqref="L12"/>
+      <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
     <col min="3" max="3" width="9.19921875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="13.1328125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A1" t="s">
         <v>3</v>
       </c>
@@ -434,8 +438,11 @@
       <c r="D1" t="s">
         <v>6</v>
       </c>
+      <c r="E1" t="s">
+        <v>7</v>
+      </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -449,8 +456,12 @@
         <f>C2+1</f>
         <v>44563</v>
       </c>
+      <c r="E2">
+        <f>B2 + 1</f>
+        <v>2</v>
+      </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A3" t="s">
         <v>1</v>
       </c>
@@ -464,8 +475,12 @@
         <f>SUM(B2:B4)</f>
         <v>6</v>
       </c>
+      <c r="E3">
+        <f t="shared" ref="E3:E4" si="0">B3 + 1</f>
+        <v>3</v>
+      </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A4" t="s">
         <v>2</v>
       </c>
@@ -478,6 +493,10 @@
       <c r="D4" t="str">
         <f>_xlfn.CONCAT(A2,A3)</f>
         <v>ab</v>
+      </c>
+      <c r="E4">
+        <f t="shared" si="0"/>
+        <v>4</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Bug: No space fail (close #6)
</commit_message>
<xml_diff>
--- a/assets/data_types.xlsx
+++ b/assets/data_types.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25427"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11010"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl.localhost\Ubuntu\home\nate\coding\excel-emulator2\assets\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/User/coding/excel-emulator2/assets/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CDD2EDD6-A39B-43FA-ACB6-DC562E8F5BC9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AC971CEB-C21A-6A41-8299-331CEAB24255}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2543" yWindow="2543" windowWidth="16875" windowHeight="10612" xr2:uid="{6F87B0DF-F7C3-4D20-8A30-9558F5F3947A}"/>
+    <workbookView xWindow="2540" yWindow="2540" windowWidth="16880" windowHeight="10620" xr2:uid="{6F87B0DF-F7C3-4D20-8A30-9558F5F3947A}"/>
   </bookViews>
   <sheets>
     <sheet name="test 1" sheetId="1" r:id="rId1"/>
@@ -29,7 +29,6 @@
         <xcalcf:feature name="microsoft.com:FV"/>
         <xcalcf:feature name="microsoft.com:CNMTM"/>
         <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -419,13 +418,13 @@
       <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="3" max="3" width="9.19921875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="13.1328125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.1640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="13.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>3</v>
       </c>
@@ -442,7 +441,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -457,11 +456,11 @@
         <v>44563</v>
       </c>
       <c r="E2">
-        <f>B2 + 1</f>
+        <f>B2+1</f>
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>1</v>
       </c>
@@ -476,11 +475,11 @@
         <v>6</v>
       </c>
       <c r="E3">
-        <f t="shared" ref="E3:E4" si="0">B3 + 1</f>
+        <f t="shared" ref="E3:E4" si="0">B3+1</f>
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>2</v>
       </c>
@@ -510,7 +509,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -522,7 +521,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>